<commit_message>
Updated sample form with Arabic
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1746EDF9-A2E3-C14D-86D5-168EBC5C596F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BE786-D85F-4043-8EF0-93F863B1CC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25940" yWindow="740" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="398">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2603,9 +2603,6 @@
     <t>intro</t>
   </si>
   <si>
-    <t>Intro</t>
-  </si>
-  <si>
     <t>custom-text-box</t>
   </si>
   <si>
@@ -2660,13 +2657,70 @@
     <t>readonly</t>
   </si>
   <si>
-    <t>This is the field plug-in with no parameters, and the field has a &lt;em&gt;default&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>SurveyCTO by Dobility</t>
+  </si>
+  <si>
+    <t>Here, the field plug-in has no parameters, the field has a &lt;em&gt;default&lt;/em&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>هذا هو الحقل الإضافي الأساسي بدون تعيين أية معلمات.</t>
+  </si>
+  <si>
+    <t>label:عربى</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+العدد الافتراضي للصفوف هو 3 لكن منطقة النص هذه بها 6 صفوف ، كما هو محدد بواسطة
+&lt;code&gt;من الصفوف&lt;/code&gt;
+معامل.
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هذا المجال لديه
+&lt;code&gt;count&lt;/code&gt;
+قيمة 1 ، لذا فهي تحسب عدد الأحرف التي تم إدخالها حتى الآن.
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هذا المجال لديه
+&lt;code&gt;max&lt;/code&gt;
+بقيمة 10، لذلك لا يمكنك إدخال أكثر من 10 أحرف (عادةً ما يكون ملف
+&lt;code&gt;max&lt;/code&gt;
+القيمة أعلى بكثير ، ولكن هذا يعمل لأغراض التوضيح).
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هنا ، لا يحتوي المكون الإضافي للحقل على معلمات ، ويحتوي الحقل على
+&lt;em&gt;
+default
+&lt;/em&gt;
+القيمة ، وهي كذلك
+&lt;em&gt; read only&lt;/ em&gt;
+(يقرأ فقط).
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>This sample form demonstrates the text-box field plug-in. You can switch to عربى to view what the field plug-in will look like in right-to-left languages (translated using Google Translate, so they will not be perfect). To learn more, check out the &lt;a href="https://github.com/surveycto/text-box/blob/main/README.md" target="_blank"&gt;readme&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هذا المجال لديه
+&lt;code&gt;count&lt;/code&gt;
+قيمة 1 ، و
+&lt;code&gt;max&lt;/code&gt;
+القيمة 10 ، لذا فهي تحسب عدد الأحرف المستخدمة حتى الآن ، ولا يمكنك إدخال أكثر من 10 أحرف.
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -4816,10 +4870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
@@ -4830,29 +4884,30 @@
     <col min="1" max="1" width="29" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" style="9" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" style="9" customWidth="1"/>
-    <col min="20" max="21" width="48" style="9" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11" style="2"/>
+    <col min="4" max="4" width="30.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="9" customWidth="1"/>
+    <col min="21" max="22" width="48" style="9" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -4862,78 +4917,81 @@
       <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -4941,84 +4999,84 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>305</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="N9" s="9" t="s">
+      <c r="K9" s="11"/>
+      <c r="O9" s="9" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="I11" s="11"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:24" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -5026,143 +5084,161 @@
         <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="F12" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+      <c r="D13" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+      <c r="D14" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="187" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="D16" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="187" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="N18" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>389</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:D1048576 J1:J1048576 G1:G1048576">
     <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 O1:O1048576 I1:I1048576">
+  <conditionalFormatting sqref="B1:D1048576 P1:P1048576 J1:J1048576">
     <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:E1048576 G1:G1048576">
     <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
+  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
     <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
+  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
     <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
     <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
+  <conditionalFormatting sqref="G1:G1048576 B1:B1048576">
     <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
@@ -5173,27 +5249,27 @@
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
+  <conditionalFormatting sqref="O1:O1048576 B1:B1048576">
     <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
     <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
     <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
+  <conditionalFormatting sqref="A1:X1048576">
     <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5257,7 +5333,7 @@
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
+  <conditionalFormatting sqref="B1:B1048576 G1:G1048576">
     <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5416,14 +5492,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>373</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>374</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2105271550</v>
+        <v>2105272010</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Updated sample form with latest parameters
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F21B46E-0522-BD48-A7CF-EE0B5A6758F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFDFC1F-2C5A-2844-A890-DA89C84483D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26400" yWindow="720" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="394">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2624,9 +2624,6 @@
     <t>six_rows</t>
   </si>
   <si>
-    <t>The default number of rows is 3 but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.</t>
-  </si>
-  <si>
     <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, so it counts the number of characters entered so far.</t>
   </si>
   <si>
@@ -2636,21 +2633,12 @@
     <t>This field has a &lt;code&gt;max&lt;/code&gt; value of 10, so you cannot enter more than 10 characters (usually, the &lt;code&gt;max&lt;/code&gt; value is a lot higher, but this works for demonstration purposes).</t>
   </si>
   <si>
-    <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, and a &lt;code&gt;max&lt;/code&gt; value of 10, so it both counts the number of characters used so far, and you cannot enter more than 10 characters.</t>
-  </si>
-  <si>
-    <t>count_max</t>
-  </si>
-  <si>
     <t>custom-text-box(rows=6)</t>
   </si>
   <si>
     <t>custom-text-box(count=1)</t>
   </si>
   <si>
-    <t>custom-text-box(count=1, max=10)</t>
-  </si>
-  <si>
     <t>custom-text-box(max=10)</t>
   </si>
   <si>
@@ -2672,35 +2660,7 @@
     <t>label:عربى</t>
   </si>
   <si>
-    <t>&lt;div dir="rtl"&gt;
-العدد الافتراضي للصفوف هو 3 لكن منطقة النص هذه بها 6 صفوف ، كما هو محدد بواسطة
-&lt;code&gt;من الصفوف&lt;/code&gt;
-معامل.
-&lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div dir="rtl"&gt;
-هذا المجال لديه
-&lt;code&gt;count&lt;/code&gt;
-قيمة 1 ، لذا فهي تحسب عدد الأحرف التي تم إدخالها حتى الآن.
-&lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>This sample form demonstrates the text-box field plug-in. You can switch to عربى to view what the field plug-in will look like in right-to-left languages (translated using Google Translate, so they will not be perfect). To learn more, check out the &lt;a href="https://github.com/surveycto/text-box/blob/main/README.md" target="_blank"&gt;readme&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;div dir="rtl"&gt;
-هنا ، لا يحتوي المكون الإضافي للحقل على معلمات، ويحتوي الحقل على
-&lt;em&gt;
-default
-&lt;/em&gt;
-القيمة، وهي كذلك
-&lt;em&gt; read only&lt;/ em&gt;
-(يقرأ فقط).
-&lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div dir="rtl"&gt;
@@ -2713,12 +2673,33 @@
 &lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
   </si>
   <si>
+    <t>The default number of rows is 3, but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+العدد الافتراضي للصفوف هو 3، لكن منطقة النص هذه بها 6 صفوف، كما هو محدد بواسطة
+&lt;code&gt;من الصفوف&lt;/code&gt;
+معامل.
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>&lt;div dir="rtl"&gt;
 هذا المجال لديه
 &lt;code&gt;count&lt;/code&gt;
-قيمة 1، و
-&lt;code&gt;max&lt;/code&gt;
-القيمة 10 ، لذا فهي تحسب عدد الأحرف المستخدمة حتى الآن، ولا يمكنك إدخال أكثر من 10 أحرف.
+قيمة 1، لذا فهي تحسب عدد الأحرف التي تم إدخالها حتى الآن.
+&lt;/div&gt;
+&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هنا، لا يحتوي المكون الإضافي للحقل على معلمات، ويحتوي الحقل على
+&lt;em&gt;
+default
+&lt;/em&gt;
+القيمة، وهي كذلك
+&lt;em&gt; read only&lt;/ em&gt;
+(يقرأ فقط).
 &lt;/div&gt;
 &lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
   </si>
@@ -4870,13 +4851,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4918,7 +4899,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
@@ -5084,7 +5065,7 @@
         <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>368</v>
@@ -5103,7 +5084,7 @@
         <v>371</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>369</v>
@@ -5117,87 +5098,70 @@
         <v>375</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="136" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="187" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="187" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="204" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="G18" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="N18" s="9" t="s">
-        <v>387</v>
+      <c r="N17" s="9" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -5499,7 +5463,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2105272026</v>
+        <v>2106031956</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Added appearances to sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFDFC1F-2C5A-2844-A890-DA89C84483D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784118A9-5A9C-EB45-AC2E-C09DECA08215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2609,9 +2609,6 @@
     <t>basic</t>
   </si>
   <si>
-    <t>This is the basic field plug-in without any parameters set.</t>
-  </si>
-  <si>
     <t>Text box sample form</t>
   </si>
   <si>
@@ -2624,15 +2621,9 @@
     <t>six_rows</t>
   </si>
   <si>
-    <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, so it counts the number of characters entered so far.</t>
-  </si>
-  <si>
     <t>max</t>
   </si>
   <si>
-    <t>This field has a &lt;code&gt;max&lt;/code&gt; value of 10, so you cannot enter more than 10 characters (usually, the &lt;code&gt;max&lt;/code&gt; value is a lot higher, but this works for demonstration purposes).</t>
-  </si>
-  <si>
     <t>custom-text-box(rows=6)</t>
   </si>
   <si>
@@ -2649,9 +2640,6 @@
   </si>
   <si>
     <t>SurveyCTO by Dobility</t>
-  </si>
-  <si>
-    <t>Here, the field plug-in has no parameters, the field has a &lt;em&gt;default&lt;/em&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.</t>
   </si>
   <si>
     <t>هذا هو الحقل الإضافي الأساسي بدون تعيين أية معلمات.</t>
@@ -2671,9 +2659,6 @@
 القيمة أعلى بكثير، ولكن هذا يعمل لأغراض التوضيح).
 &lt;/div&gt;
 &lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>The default number of rows is 3, but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.</t>
   </si>
   <si>
     <t>&lt;div dir="rtl"&gt;
@@ -2702,6 +2687,31 @@
 (يقرأ فقط).
 &lt;/div&gt;
 &lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>This field has a &lt;code&gt;max&lt;/code&gt; value of 10, so you cannot enter more than 10 characters (usually, the &lt;code&gt;max&lt;/code&gt; value is a lot higher, but this works for demonstration purposes).&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(max=10)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>This is the basic field plug-in without any parameters set.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>The default number of rows is 3, but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(rows=6)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, so it counts the number of characters entered so far.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(count=1)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>Here, the field plug-in has no parameters, the field has a &lt;em&gt;default&lt;/em&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box&lt;/code&gt;</t>
   </si>
 </sst>
 </file>
@@ -4854,7 +4864,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
@@ -4899,7 +4909,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
@@ -5065,7 +5075,7 @@
         <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>368</v>
@@ -5073,7 +5083,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
@@ -5081,10 +5091,10 @@
         <v>370</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>369</v>
@@ -5095,16 +5105,16 @@
         <v>96</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="187" x14ac:dyDescent="0.2">
@@ -5112,16 +5122,16 @@
         <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>378</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="136" x14ac:dyDescent="0.2">
@@ -5129,16 +5139,16 @@
         <v>96</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="204" x14ac:dyDescent="0.2">
@@ -5146,22 +5156,22 @@
         <v>96</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>369</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -5456,14 +5466,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>373</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2106031956</v>
+        <v>2106042150</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Changed alignment of appearances
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784118A9-5A9C-EB45-AC2E-C09DECA08215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6611335D-6650-714E-9457-65BA792EF452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27040" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2642,13 +2642,55 @@
     <t>SurveyCTO by Dobility</t>
   </si>
   <si>
-    <t>هذا هو الحقل الإضافي الأساسي بدون تعيين أية معلمات.</t>
-  </si>
-  <si>
     <t>label:عربى</t>
   </si>
   <si>
     <t>This sample form demonstrates the text-box field plug-in. You can switch to عربى to view what the field plug-in will look like in right-to-left languages (translated using Google Translate, so they will not be perfect). To learn more, check out the &lt;a href="https://github.com/surveycto/text-box/blob/main/README.md" target="_blank"&gt;readme&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>This field has a &lt;code&gt;max&lt;/code&gt; value of 10, so you cannot enter more than 10 characters (usually, the &lt;code&gt;max&lt;/code&gt; value is a lot higher, but this works for demonstration purposes).&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(max=10)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>This is the basic field plug-in without any parameters set.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>The default number of rows is 3, but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(rows=6)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, so it counts the number of characters entered so far.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(count=1)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>Here, the field plug-in has no parameters, the field has a &lt;em&gt;default&lt;/em&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هذا هو الحقل الإضافي الأساسي بدون تعيين أية معلمات.
+&lt;/div&gt;
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box&lt;/code&gt;
+&lt;/dir&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+العدد الافتراضي للصفوف هو 3، لكن منطقة النص هذه بها 6 صفوف، كما هو محدد بواسطة
+&lt;code&gt;من الصفوف&lt;/code&gt;
+معامل.
+&lt;/div&gt;
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box(rows=6)&lt;/code&gt;
+&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div dir="rtl"&gt;
@@ -2658,15 +2700,10 @@
 &lt;code&gt;max&lt;/code&gt;
 القيمة أعلى بكثير، ولكن هذا يعمل لأغراض التوضيح).
 &lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div dir="rtl"&gt;
-العدد الافتراضي للصفوف هو 3، لكن منطقة النص هذه بها 6 صفوف، كما هو محدد بواسطة
-&lt;code&gt;من الصفوف&lt;/code&gt;
-معامل.
-&lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box(max=10)&lt;/code&gt;
+&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div dir="rtl"&gt;
@@ -2674,7 +2711,10 @@
 &lt;code&gt;count&lt;/code&gt;
 قيمة 1، لذا فهي تحسب عدد الأحرف التي تم إدخالها حتى الآن.
 &lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box(count=1)&lt;/code&gt;
+&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div dir="rtl"&gt;
@@ -2683,35 +2723,13 @@
 default
 &lt;/em&gt;
 القيمة، وهي كذلك
-&lt;em&gt; read only&lt;/ em&gt;
+&lt;em&gt;read only&lt;/em&gt;
 (يقرأ فقط).
 &lt;/div&gt;
-&lt;div style="line-height:0"&gt;&lt;br&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>This field has a &lt;code&gt;max&lt;/code&gt; value of 10, so you cannot enter more than 10 characters (usually, the &lt;code&gt;max&lt;/code&gt; value is a lot higher, but this works for demonstration purposes).&lt;br&gt;
+&lt;div dir="rtl"&gt;
 &lt;br&gt;
-&lt;code&gt;custom-text-box(max=10)&lt;/code&gt;</t>
-  </si>
-  <si>
-    <t>This is the basic field plug-in without any parameters set.&lt;br&gt;
-&lt;br&gt;
-&lt;code&gt;custom-text-box&lt;/code&gt;</t>
-  </si>
-  <si>
-    <t>The default number of rows is 3, but this text area has 6 rows, as determined by the &lt;code&gt;rows&lt;/code&gt; parameter.&lt;br&gt;
-&lt;br&gt;
-&lt;code&gt;custom-text-box(rows=6)&lt;/code&gt;</t>
-  </si>
-  <si>
-    <t>This field has a &lt;code&gt;count&lt;/code&gt; value of 1, so it counts the number of characters entered so far.&lt;br&gt;
-&lt;br&gt;
-&lt;code&gt;custom-text-box(count=1)&lt;/code&gt;</t>
-  </si>
-  <si>
-    <t>Here, the field plug-in has no parameters, the field has a &lt;em&gt;default&lt;/em&gt; value, and it is &lt;em&gt;read only&lt;/em&gt;.&lt;br&gt;
-&lt;br&gt;
-&lt;code&gt;custom-text-box&lt;/code&gt;</t>
+&lt;code&gt;custom-text-box&lt;/code&gt;
+&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -4909,7 +4927,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
@@ -5075,7 +5093,7 @@
         <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>368</v>
@@ -5083,7 +5101,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
@@ -5091,16 +5109,16 @@
         <v>370</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="153" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="204" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>96</v>
       </c>
@@ -5108,16 +5126,16 @@
         <v>374</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="187" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>96</v>
       </c>
@@ -5125,16 +5143,16 @@
         <v>375</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="136" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="187" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>96</v>
       </c>
@@ -5142,16 +5160,16 @@
         <v>373</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>392</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>387</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>96</v>
       </c>
@@ -5159,10 +5177,10 @@
         <v>379</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>393</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>388</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>381</v>
@@ -5473,7 +5491,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2106042150</v>
+        <v>2106042204</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Updated sample form with more demos
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6611335D-6650-714E-9457-65BA792EF452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA54E15F-FD8B-EC41-85A1-CFB2BC25025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27040" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="help-choices" sheetId="5" r:id="rId5"/>
     <sheet name="help-settings" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="402">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2730,6 +2730,34 @@
 &lt;br&gt;
 &lt;code&gt;custom-text-box&lt;/code&gt;
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>no_fpi</t>
+  </si>
+  <si>
+    <t>expand</t>
+  </si>
+  <si>
+    <t>custom-text-box(expand=1)</t>
+  </si>
+  <si>
+    <t>expand_limit</t>
+  </si>
+  <si>
+    <t>This text box also expands, but only until a certain point. The &lt;code&gt;rows&lt;/code&gt; parameter normally defines the number of rows shown, but when used with the &lt;code&gt;expand&lt;/code&gt; parameter, it defines at how many rows to stop expanding the text input area.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(expand=1, rows=5)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>custom-text-box(expand=1, rows=5)</t>
+  </si>
+  <si>
+    <t>This field has no field plug-in, so you can compare it to the field plug-in.</t>
+  </si>
+  <si>
+    <t>Here, the text box expands to fit its contents, just like fields without field plug-ins.&lt;br&gt;
+&lt;br&gt;
+&lt;code&gt;custom-text-box(expand=1)&lt;/code&gt;</t>
   </si>
 </sst>
 </file>
@@ -4879,13 +4907,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5101,94 +5129,135 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:24" ht="136" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="204" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="238" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="187" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="238" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="187" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N20" s="9" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5491,7 +5560,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2106042204</v>
+        <v>2106092316</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Updated form with Arabic
</commit_message>
<xml_diff>
--- a/extras/sample-form/Text box sample form.xlsx
+++ b/extras/sample-form/Text box sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-box/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA54E15F-FD8B-EC41-85A1-CFB2BC25025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B8812-2CD8-D744-ACAB-F09321AA8FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27040" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="406">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2755,9 +2755,43 @@
     <t>This field has no field plug-in, so you can compare it to the field plug-in.</t>
   </si>
   <si>
-    <t>Here, the text box expands to fit its contents, just like fields without field plug-ins.&lt;br&gt;
+    <t>&lt;div dir="rtl"&gt;
+يوضح هذا النموذج النموذجي المكون الإضافي لحقل مربع النص. يمكنك التبديل إلى english لعرض الشكل الذي سيبدو عليه المكون الإضافي الميداني باللغات التي تُكتب من اليمين إلى اليسار (تمت ترجمتها باستخدام الترجمة من Google ، لذا لن تكون مثالية). لمعرفة المزيد ، راجع &lt;a href="https://github.com/surveycto/text-box/blob/main/README.md" target="_blank"&gt; الملف التمهيدي &lt;/a&gt;.
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+لا يحتوي هذا الحقل على حقل إضافي ، لذا يمكنك مقارنته بالمكون الإضافي للحقل.
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Here, the &lt;code&gt;expand&lt;/code&gt; parameter has a value of 1, so the text box expands to fit its contents, just like fields without field plug-ins.&lt;br&gt;
 &lt;br&gt;
 &lt;code&gt;custom-text-box(expand=1)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+يتوسع مربع النص هذا أيضًا، ولكن فقط حتى نقطة معينة. ال
+&lt;code&gt;rows&lt;/code&gt;
+تحدد المعلمة عادةً عدد الصفوف المعروضة، ولكن عند استخدامها مع
+&lt;code&gt;expand&lt;/code&gt;
+المعلمة، فهي تحدد عدد الصفوف التي يجب إيقاف توسيع منطقة إدخال النص فيها
+&lt;/div&gt;
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box(expand=1, rows=5)&lt;/code&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div dir="rtl"&gt;
+هنا،
+&lt;code&gt;expand&lt;/code&gt;
+المعلمة لها قيمة 1، لذلك يتم توسيع مربع النص ليلائم محتوياته ، تمامًا مثل الحقول التي لا تحتوي على مكونات إضافية للحقل.
+&lt;/div&gt;
+&lt;br&gt;
+&lt;div dir="rtl"&gt;
+&lt;code&gt;custom-text-box(expand=1)&lt;/code&gt;
+&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -5113,7 +5147,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:24" ht="204" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -5123,13 +5157,16 @@
       <c r="C12" s="10" t="s">
         <v>383</v>
       </c>
+      <c r="D12" s="10" t="s">
+        <v>401</v>
+      </c>
       <c r="G12" s="9" t="s">
         <v>368</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
@@ -5138,6 +5175,9 @@
       </c>
       <c r="C13" s="10" t="s">
         <v>400</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>402</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -5210,7 +5250,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>96</v>
       </c>
@@ -5218,13 +5258,16 @@
         <v>395</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>401</v>
+        <v>403</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>405</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>96</v>
       </c>
@@ -5233,6 +5276,9 @@
       </c>
       <c r="C19" s="10" t="s">
         <v>398</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>404</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>399</v>
@@ -5560,7 +5606,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2106092316</v>
+        <v>2106112018</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>